<commit_message>
add ansible_palubook use method   and  linux use tips
</commit_message>
<xml_diff>
--- a/python/python.xlsx
+++ b/python/python.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>列表，元组，字典</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -693,6 +693,54 @@
   </si>
   <si>
     <t xml:space="preserve">socket </t>
+  </si>
+  <si>
+    <r>
+      <t>ftplib</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>FTP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>模块</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>thread</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_thread</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>threading</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -775,7 +823,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -792,6 +840,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1154,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1433,6 +1482,31 @@
     <row r="51" spans="1:1">
       <c r="A51" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="8">
+        <v>43580</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>